<commit_message>
phân công nhiệm vụ
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duycs\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Chuyên đề\CD-Team07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269A0B8C-8ECC-417C-9315-734B7BD5503C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{4583C4E1-F2DA-44C2-8048-959C56D65FD0}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Triển khai hệ thống</t>
   </si>
@@ -119,11 +118,44 @@
   <si>
     <t>`</t>
   </si>
+  <si>
+    <t>Phân công nhiệm vụ</t>
+  </si>
+  <si>
+    <t>Cả nhóm cùng họp lại, lập kế hoạch cụ thể. Trưởng nhóm phân công nhiệm vụ tạm thời cho từng thành viên</t>
+  </si>
+  <si>
+    <t>Dựa vào nhiệm vụ tạm thời, từng thành viên tự xác định tiến độ công việc</t>
+  </si>
+  <si>
+    <t>Trưởng nhóm phê duyệt tiến độ dự kiến, điều chỉnh kế hoạch</t>
+  </si>
+  <si>
+    <t>Minh Tuấn thực hiện</t>
+  </si>
+  <si>
+    <t>Khương Duy, Bắc Việt thực hiện</t>
+  </si>
+  <si>
+    <t>Kiên Trung, Khương Duy, Bắc Việt thực hiện</t>
+  </si>
+  <si>
+    <t>Quang Tạo thực hiện</t>
+  </si>
+  <si>
+    <t>Tất cả thành viên đều tham gia lập trình</t>
+  </si>
+  <si>
+    <t>Bắc Việt thực hiện</t>
+  </si>
+  <si>
+    <t>Minh Tuấn, Bắc Việt thực hiện</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -248,17 +280,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -310,11 +331,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -328,9 +360,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -343,7 +372,7 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -358,25 +387,37 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -385,46 +426,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -740,687 +775,734 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA8D7113-DA04-4B0D-96D7-EDFCBE6E656C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="Y19" sqref="Y19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.3671875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="6.20703125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="6.3671875" style="7" customWidth="1"/>
-    <col min="4" max="5" width="6.20703125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="6.1015625" style="7" customWidth="1"/>
-    <col min="7" max="8" width="6.3125" style="7" customWidth="1"/>
-    <col min="9" max="10" width="6.578125" style="7" customWidth="1"/>
-    <col min="11" max="11" width="6.20703125" style="7" customWidth="1"/>
-    <col min="12" max="12" width="6.15625" style="7" customWidth="1"/>
-    <col min="13" max="13" width="6.3671875" style="7" customWidth="1"/>
-    <col min="14" max="14" width="6.26171875" style="7" customWidth="1"/>
-    <col min="15" max="15" width="6.20703125" style="7" customWidth="1"/>
-    <col min="16" max="16" width="6.26171875" style="7" customWidth="1"/>
-    <col min="17" max="17" width="6.41796875" style="7" customWidth="1"/>
-    <col min="18" max="18" width="6.20703125" style="7" customWidth="1"/>
-    <col min="19" max="19" width="6.15625" style="7" customWidth="1"/>
-    <col min="20" max="20" width="6.20703125" style="7" customWidth="1"/>
-    <col min="21" max="16384" width="8.83984375" style="7"/>
+    <col min="1" max="1" width="10.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="6.21875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" style="6" customWidth="1"/>
+    <col min="4" max="5" width="6.21875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="6.109375" style="6" customWidth="1"/>
+    <col min="7" max="8" width="6.33203125" style="6" customWidth="1"/>
+    <col min="9" max="10" width="6.5546875" style="6" customWidth="1"/>
+    <col min="11" max="11" width="6.21875" style="6" customWidth="1"/>
+    <col min="12" max="12" width="6.109375" style="6" customWidth="1"/>
+    <col min="13" max="13" width="6.33203125" style="6" customWidth="1"/>
+    <col min="14" max="16" width="6.21875" style="6" customWidth="1"/>
+    <col min="17" max="17" width="6.44140625" style="6" customWidth="1"/>
+    <col min="18" max="18" width="6.21875" style="6" customWidth="1"/>
+    <col min="19" max="19" width="6.109375" style="6" customWidth="1"/>
+    <col min="20" max="20" width="6.21875" style="6" customWidth="1"/>
+    <col min="21" max="21" width="8.88671875" style="6"/>
+    <col min="22" max="22" width="44.44140625" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="8">
+    <row r="1" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7">
         <v>44256</v>
       </c>
-      <c r="B1" s="9">
+      <c r="B1" s="8">
         <v>44263</v>
       </c>
-      <c r="C1" s="9">
+      <c r="C1" s="8">
         <v>44270</v>
       </c>
-      <c r="D1" s="9">
+      <c r="D1" s="8">
         <v>44277</v>
       </c>
-      <c r="E1" s="9">
+      <c r="E1" s="8">
         <v>44284</v>
       </c>
-      <c r="F1" s="9">
+      <c r="F1" s="8">
         <v>44291</v>
       </c>
-      <c r="G1" s="9">
+      <c r="G1" s="8">
         <v>44298</v>
       </c>
-      <c r="H1" s="9">
+      <c r="H1" s="8">
         <v>44305</v>
       </c>
-      <c r="I1" s="9">
+      <c r="I1" s="8">
         <v>44312</v>
       </c>
-      <c r="J1" s="9">
+      <c r="J1" s="8">
         <v>44319</v>
       </c>
-      <c r="K1" s="9">
+      <c r="K1" s="8">
         <v>44326</v>
       </c>
-      <c r="L1" s="9">
+      <c r="L1" s="8">
         <v>44333</v>
       </c>
-      <c r="M1" s="9">
+      <c r="M1" s="8">
         <v>44340</v>
       </c>
-      <c r="N1" s="9">
+      <c r="N1" s="8">
         <v>44347</v>
       </c>
-      <c r="O1" s="9">
+      <c r="O1" s="8">
         <v>44354</v>
       </c>
-      <c r="P1" s="9">
+      <c r="P1" s="8">
         <v>44361</v>
       </c>
-      <c r="Q1" s="9">
+      <c r="Q1" s="8">
         <v>44368</v>
       </c>
-      <c r="R1" s="9">
+      <c r="R1" s="8">
         <v>44375</v>
       </c>
-      <c r="S1" s="9">
+      <c r="S1" s="8">
         <v>44382</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="34.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:22" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>1</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>2</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>3</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>4</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>5</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>6</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <v>7</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="5">
         <v>8</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="5">
         <v>9</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="5">
         <v>10</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="5">
         <v>11</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="5">
         <v>12</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="5">
         <v>13</v>
       </c>
-      <c r="O2" s="6">
+      <c r="O2" s="5">
         <v>14</v>
       </c>
-      <c r="P2" s="6">
+      <c r="P2" s="5">
         <v>15</v>
       </c>
-      <c r="Q2" s="6">
+      <c r="Q2" s="5">
         <v>16</v>
       </c>
-      <c r="R2" s="6">
+      <c r="R2" s="5">
         <v>17</v>
       </c>
-      <c r="S2" s="6">
+      <c r="S2" s="5">
         <v>18</v>
       </c>
-      <c r="T2" s="6">
+      <c r="T2" s="5">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="11" t="str">
+      <c r="B3" s="10" t="str">
         <f>TEXT(A1,"dd/mm/yyyy")</f>
         <v>01/03/2021</v>
       </c>
-      <c r="C3" s="11" t="str">
+      <c r="C3" s="10" t="str">
         <f t="shared" ref="C3:D3" si="0">TEXT(B1,"dd/mm/yyyy")</f>
         <v>08/03/2021</v>
       </c>
-      <c r="D3" s="11" t="str">
+      <c r="D3" s="10" t="str">
         <f t="shared" si="0"/>
         <v>15/03/2021</v>
       </c>
-      <c r="E3" s="11" t="str">
+      <c r="E3" s="10" t="str">
         <f t="shared" ref="E3:T3" si="1">TEXT(D1,"dd/mm/yyyy")</f>
         <v>22/03/2021</v>
       </c>
-      <c r="F3" s="11" t="str">
+      <c r="F3" s="10" t="str">
         <f t="shared" si="1"/>
         <v>29/03/2021</v>
       </c>
-      <c r="G3" s="11" t="str">
+      <c r="G3" s="10" t="str">
         <f t="shared" si="1"/>
         <v>05/04/2021</v>
       </c>
-      <c r="H3" s="11" t="str">
+      <c r="H3" s="10" t="str">
         <f t="shared" si="1"/>
         <v>12/04/2021</v>
       </c>
-      <c r="I3" s="11" t="str">
+      <c r="I3" s="10" t="str">
         <f t="shared" si="1"/>
         <v>19/04/2021</v>
       </c>
-      <c r="J3" s="11" t="str">
+      <c r="J3" s="10" t="str">
         <f t="shared" si="1"/>
         <v>26/04/2021</v>
       </c>
-      <c r="K3" s="11" t="str">
+      <c r="K3" s="10" t="str">
         <f t="shared" si="1"/>
         <v>03/05/2021</v>
       </c>
-      <c r="L3" s="11" t="str">
+      <c r="L3" s="10" t="str">
         <f t="shared" si="1"/>
         <v>10/05/2021</v>
       </c>
-      <c r="M3" s="11" t="str">
+      <c r="M3" s="10" t="str">
         <f t="shared" si="1"/>
         <v>17/05/2021</v>
       </c>
-      <c r="N3" s="11" t="str">
+      <c r="N3" s="10" t="str">
         <f t="shared" si="1"/>
         <v>24/05/2021</v>
       </c>
-      <c r="O3" s="11" t="str">
+      <c r="O3" s="10" t="str">
         <f t="shared" si="1"/>
         <v>31/05/2021</v>
       </c>
-      <c r="P3" s="11" t="str">
+      <c r="P3" s="10" t="str">
         <f t="shared" si="1"/>
         <v>07/06/2021</v>
       </c>
-      <c r="Q3" s="11" t="str">
+      <c r="Q3" s="10" t="str">
         <f t="shared" si="1"/>
         <v>14/06/2021</v>
       </c>
-      <c r="R3" s="11" t="str">
+      <c r="R3" s="10" t="str">
         <f t="shared" si="1"/>
         <v>21/06/2021</v>
       </c>
-      <c r="S3" s="11" t="str">
+      <c r="S3" s="10" t="str">
         <f t="shared" si="1"/>
         <v>28/06/2021</v>
       </c>
-      <c r="T3" s="11" t="str">
+      <c r="T3" s="10" t="str">
         <f t="shared" si="1"/>
         <v>05/07/2021</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="3" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="35" t="s">
+    <row r="4" spans="1:22" s="3" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="21" t="s">
+      <c r="C4" s="33"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="24" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" s="3" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33" t="s">
+      <c r="V4" s="35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" s="3" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="22"/>
-    </row>
-    <row r="6" spans="1:20" s="3" customFormat="1" ht="30.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="33"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="33" t="s">
+      <c r="C5" s="18"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="25"/>
+      <c r="V5" s="35"/>
+    </row>
+    <row r="6" spans="1:22" s="3" customFormat="1" ht="30.3" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="22"/>
-    </row>
-    <row r="7" spans="1:20" s="3" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="33"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="33" t="s">
+      <c r="D6" s="16"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="25"/>
+      <c r="V6" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" s="3" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="16"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="22"/>
-    </row>
-    <row r="8" spans="1:20" s="3" customFormat="1" ht="35.700000000000003" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="33"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="33" t="s">
+      <c r="D7" s="16"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="25"/>
+      <c r="V7" s="2"/>
+    </row>
+    <row r="8" spans="1:22" s="3" customFormat="1" ht="35.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="22"/>
-    </row>
-    <row r="9" spans="1:20" s="3" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="36" t="s">
+      <c r="D8" s="18"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="25"/>
+      <c r="V8" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" s="3" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="36" t="s">
+      <c r="B9" s="23"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="22"/>
-    </row>
-    <row r="10" spans="1:20" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="36"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="36" t="s">
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="25"/>
+      <c r="V9" s="35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="17"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="22"/>
-    </row>
-    <row r="11" spans="1:20" s="3" customFormat="1" ht="45.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="36"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="36" t="s">
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="25"/>
+      <c r="V10" s="35"/>
+    </row>
+    <row r="11" spans="1:22" s="3" customFormat="1" ht="45.3" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="17"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="37"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="22"/>
-    </row>
-    <row r="12" spans="1:20" s="3" customFormat="1" ht="21.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="31" t="s">
+      <c r="F11" s="19"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="25"/>
+      <c r="V11" s="35"/>
+    </row>
+    <row r="12" spans="1:22" s="3" customFormat="1" ht="21.3" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="31" t="s">
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="17"/>
-      <c r="S12" s="17"/>
-      <c r="T12" s="22"/>
-    </row>
-    <row r="13" spans="1:20" s="3" customFormat="1" ht="31.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="31"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="31" t="s">
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="25"/>
+      <c r="V12" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" s="3" customFormat="1" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="20"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="17"/>
-      <c r="T13" s="22"/>
-    </row>
-    <row r="14" spans="1:20" s="3" customFormat="1" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="31"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="31" t="s">
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23"/>
+      <c r="T13" s="25"/>
+      <c r="V13" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" s="3" customFormat="1" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="20"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="H14" s="31"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="22"/>
-    </row>
-    <row r="15" spans="1:20" s="3" customFormat="1" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="31"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="31" t="s">
+      <c r="H14" s="20"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23"/>
+      <c r="T14" s="25"/>
+      <c r="V14" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" s="3" customFormat="1" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="20"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="31"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-      <c r="T15" s="22"/>
-    </row>
-    <row r="16" spans="1:20" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="13" t="s">
+      <c r="H15" s="20"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="25"/>
+      <c r="V15" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="25" t="s">
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
-      <c r="T16" s="22"/>
-    </row>
-    <row r="17" spans="1:23" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="14" t="s">
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="25"/>
+      <c r="V16" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="26" t="s">
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="N17" s="26"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
-      <c r="T17" s="22"/>
-    </row>
-    <row r="18" spans="1:23" s="3" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="28" t="s">
+      <c r="N17" s="31"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="25"/>
+      <c r="V17" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" s="3" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="28" t="s">
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="R18" s="28"/>
-      <c r="S18" s="29"/>
-      <c r="T18" s="22"/>
-    </row>
-    <row r="19" spans="1:23" s="3" customFormat="1" ht="82.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="28"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="15" t="s">
+      <c r="R18" s="21"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="25"/>
+      <c r="V18" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" s="3" customFormat="1" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="21"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="22"/>
-    </row>
-    <row r="20" spans="1:23" s="3" customFormat="1" ht="30.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="28"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="30" t="s">
+      <c r="R19" s="37"/>
+      <c r="S19" s="38"/>
+      <c r="T19" s="25"/>
+      <c r="V19" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" s="3" customFormat="1" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="21"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="R20" s="30"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="22"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="25"/>
+      <c r="V20" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="W20" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:23" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="16" t="s">
+    <row r="21" spans="1:23" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A21" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="23"/>
-      <c r="Q21" s="23"/>
-      <c r="R21" s="23"/>
-      <c r="S21" s="23"/>
-      <c r="T21" s="22"/>
-    </row>
-    <row r="22" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="26"/>
+      <c r="R21" s="26"/>
+      <c r="S21" s="26"/>
+      <c r="T21" s="25"/>
+      <c r="V21" s="2"/>
+    </row>
+    <row r="22" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1441,8 +1523,9 @@
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
-    </row>
-    <row r="23" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V22" s="2"/>
+    </row>
+    <row r="23" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1463,8 +1546,9 @@
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
-    </row>
-    <row r="24" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V23" s="2"/>
+    </row>
+    <row r="24" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1485,8 +1569,9 @@
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
-    </row>
-    <row r="25" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V24" s="2"/>
+    </row>
+    <row r="25" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1507,8 +1592,9 @@
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
-    </row>
-    <row r="26" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V25" s="2"/>
+    </row>
+    <row r="26" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1529,8 +1615,9 @@
       <c r="R26" s="2"/>
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
-    </row>
-    <row r="27" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V26" s="2"/>
+    </row>
+    <row r="27" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1551,8 +1638,9 @@
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
-    </row>
-    <row r="28" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V27" s="2"/>
+    </row>
+    <row r="28" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1573,8 +1661,9 @@
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
-    </row>
-    <row r="29" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V28" s="2"/>
+    </row>
+    <row r="29" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1595,8 +1684,9 @@
       <c r="R29" s="2"/>
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
-    </row>
-    <row r="30" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V29" s="2"/>
+    </row>
+    <row r="30" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1617,8 +1707,9 @@
       <c r="R30" s="2"/>
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
-    </row>
-    <row r="31" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V30" s="2"/>
+    </row>
+    <row r="31" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1639,8 +1730,9 @@
       <c r="R31" s="2"/>
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
-    </row>
-    <row r="32" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V31" s="2"/>
+    </row>
+    <row r="32" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1661,8 +1753,9 @@
       <c r="R32" s="2"/>
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
-    </row>
-    <row r="33" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V32" s="2"/>
+    </row>
+    <row r="33" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1683,8 +1776,9 @@
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>
       <c r="T33" s="2"/>
-    </row>
-    <row r="34" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V33" s="2"/>
+    </row>
+    <row r="34" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1705,8 +1799,9 @@
       <c r="R34" s="2"/>
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>
-    </row>
-    <row r="35" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V34" s="2"/>
+    </row>
+    <row r="35" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1727,8 +1822,9 @@
       <c r="R35" s="2"/>
       <c r="S35" s="2"/>
       <c r="T35" s="2"/>
-    </row>
-    <row r="36" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V35" s="2"/>
+    </row>
+    <row r="36" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1749,8 +1845,9 @@
       <c r="R36" s="2"/>
       <c r="S36" s="2"/>
       <c r="T36" s="2"/>
-    </row>
-    <row r="37" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V36" s="2"/>
+    </row>
+    <row r="37" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1771,8 +1868,9 @@
       <c r="R37" s="2"/>
       <c r="S37" s="2"/>
       <c r="T37" s="2"/>
-    </row>
-    <row r="38" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V37" s="2"/>
+    </row>
+    <row r="38" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1793,8 +1891,9 @@
       <c r="R38" s="2"/>
       <c r="S38" s="2"/>
       <c r="T38" s="2"/>
-    </row>
-    <row r="39" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V38" s="2"/>
+    </row>
+    <row r="39" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1815,8 +1914,9 @@
       <c r="R39" s="2"/>
       <c r="S39" s="2"/>
       <c r="T39" s="2"/>
-    </row>
-    <row r="40" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V39" s="2"/>
+    </row>
+    <row r="40" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1837,8 +1937,9 @@
       <c r="R40" s="2"/>
       <c r="S40" s="2"/>
       <c r="T40" s="2"/>
-    </row>
-    <row r="41" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V40" s="2"/>
+    </row>
+    <row r="41" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1859,8 +1960,9 @@
       <c r="R41" s="2"/>
       <c r="S41" s="2"/>
       <c r="T41" s="2"/>
-    </row>
-    <row r="42" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V41" s="2"/>
+    </row>
+    <row r="42" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1881,8 +1983,9 @@
       <c r="R42" s="2"/>
       <c r="S42" s="2"/>
       <c r="T42" s="2"/>
-    </row>
-    <row r="43" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V42" s="2"/>
+    </row>
+    <row r="43" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1903,8 +2006,9 @@
       <c r="R43" s="2"/>
       <c r="S43" s="2"/>
       <c r="T43" s="2"/>
-    </row>
-    <row r="44" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V43" s="2"/>
+    </row>
+    <row r="44" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1925,8 +2029,9 @@
       <c r="R44" s="2"/>
       <c r="S44" s="2"/>
       <c r="T44" s="2"/>
-    </row>
-    <row r="45" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V44" s="2"/>
+    </row>
+    <row r="45" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1947,8 +2052,9 @@
       <c r="R45" s="2"/>
       <c r="S45" s="2"/>
       <c r="T45" s="2"/>
-    </row>
-    <row r="46" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V45" s="2"/>
+    </row>
+    <row r="46" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1969,8 +2075,9 @@
       <c r="R46" s="2"/>
       <c r="S46" s="2"/>
       <c r="T46" s="2"/>
-    </row>
-    <row r="47" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V46" s="2"/>
+    </row>
+    <row r="47" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1991,8 +2098,9 @@
       <c r="R47" s="2"/>
       <c r="S47" s="2"/>
       <c r="T47" s="2"/>
-    </row>
-    <row r="48" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V47" s="2"/>
+    </row>
+    <row r="48" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2013,8 +2121,9 @@
       <c r="R48" s="2"/>
       <c r="S48" s="2"/>
       <c r="T48" s="2"/>
-    </row>
-    <row r="49" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V48" s="2"/>
+    </row>
+    <row r="49" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -2035,8 +2144,9 @@
       <c r="R49" s="2"/>
       <c r="S49" s="2"/>
       <c r="T49" s="2"/>
-    </row>
-    <row r="50" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V49" s="2"/>
+    </row>
+    <row r="50" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2057,8 +2167,9 @@
       <c r="R50" s="2"/>
       <c r="S50" s="2"/>
       <c r="T50" s="2"/>
-    </row>
-    <row r="51" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V50" s="2"/>
+    </row>
+    <row r="51" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -2079,8 +2190,9 @@
       <c r="R51" s="2"/>
       <c r="S51" s="2"/>
       <c r="T51" s="2"/>
-    </row>
-    <row r="52" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V51" s="2"/>
+    </row>
+    <row r="52" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -2101,8 +2213,9 @@
       <c r="R52" s="2"/>
       <c r="S52" s="2"/>
       <c r="T52" s="2"/>
-    </row>
-    <row r="53" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V52" s="2"/>
+    </row>
+    <row r="53" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -2123,8 +2236,9 @@
       <c r="R53" s="2"/>
       <c r="S53" s="2"/>
       <c r="T53" s="2"/>
-    </row>
-    <row r="54" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V53" s="2"/>
+    </row>
+    <row r="54" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2145,8 +2259,9 @@
       <c r="R54" s="2"/>
       <c r="S54" s="2"/>
       <c r="T54" s="2"/>
-    </row>
-    <row r="55" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V54" s="2"/>
+    </row>
+    <row r="55" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -2167,8 +2282,9 @@
       <c r="R55" s="2"/>
       <c r="S55" s="2"/>
       <c r="T55" s="2"/>
-    </row>
-    <row r="56" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V55" s="2"/>
+    </row>
+    <row r="56" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -2189,8 +2305,9 @@
       <c r="R56" s="2"/>
       <c r="S56" s="2"/>
       <c r="T56" s="2"/>
-    </row>
-    <row r="57" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V56" s="2"/>
+    </row>
+    <row r="57" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -2211,8 +2328,9 @@
       <c r="R57" s="2"/>
       <c r="S57" s="2"/>
       <c r="T57" s="2"/>
-    </row>
-    <row r="58" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V57" s="2"/>
+    </row>
+    <row r="58" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -2233,8 +2351,9 @@
       <c r="R58" s="2"/>
       <c r="S58" s="2"/>
       <c r="T58" s="2"/>
-    </row>
-    <row r="59" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V58" s="2"/>
+    </row>
+    <row r="59" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2255,8 +2374,9 @@
       <c r="R59" s="2"/>
       <c r="S59" s="2"/>
       <c r="T59" s="2"/>
-    </row>
-    <row r="60" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V59" s="2"/>
+    </row>
+    <row r="60" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2277,8 +2397,9 @@
       <c r="R60" s="2"/>
       <c r="S60" s="2"/>
       <c r="T60" s="2"/>
-    </row>
-    <row r="61" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V60" s="2"/>
+    </row>
+    <row r="61" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2299,8 +2420,9 @@
       <c r="R61" s="2"/>
       <c r="S61" s="2"/>
       <c r="T61" s="2"/>
-    </row>
-    <row r="62" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V61" s="2"/>
+    </row>
+    <row r="62" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2321,8 +2443,9 @@
       <c r="R62" s="2"/>
       <c r="S62" s="2"/>
       <c r="T62" s="2"/>
-    </row>
-    <row r="63" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V62" s="2"/>
+    </row>
+    <row r="63" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2343,8 +2466,9 @@
       <c r="R63" s="2"/>
       <c r="S63" s="2"/>
       <c r="T63" s="2"/>
-    </row>
-    <row r="64" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V63" s="2"/>
+    </row>
+    <row r="64" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2365,8 +2489,9 @@
       <c r="R64" s="2"/>
       <c r="S64" s="2"/>
       <c r="T64" s="2"/>
-    </row>
-    <row r="65" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V64" s="2"/>
+    </row>
+    <row r="65" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2387,8 +2512,9 @@
       <c r="R65" s="2"/>
       <c r="S65" s="2"/>
       <c r="T65" s="2"/>
-    </row>
-    <row r="66" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V65" s="2"/>
+    </row>
+    <row r="66" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2409,8 +2535,9 @@
       <c r="R66" s="2"/>
       <c r="S66" s="2"/>
       <c r="T66" s="2"/>
-    </row>
-    <row r="67" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V66" s="2"/>
+    </row>
+    <row r="67" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2431,8 +2558,9 @@
       <c r="R67" s="2"/>
       <c r="S67" s="2"/>
       <c r="T67" s="2"/>
-    </row>
-    <row r="68" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V67" s="2"/>
+    </row>
+    <row r="68" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2453,8 +2581,9 @@
       <c r="R68" s="2"/>
       <c r="S68" s="2"/>
       <c r="T68" s="2"/>
-    </row>
-    <row r="69" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V68" s="2"/>
+    </row>
+    <row r="69" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2475,8 +2604,9 @@
       <c r="R69" s="2"/>
       <c r="S69" s="2"/>
       <c r="T69" s="2"/>
-    </row>
-    <row r="70" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V69" s="2"/>
+    </row>
+    <row r="70" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2497,8 +2627,9 @@
       <c r="R70" s="2"/>
       <c r="S70" s="2"/>
       <c r="T70" s="2"/>
-    </row>
-    <row r="71" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V70" s="2"/>
+    </row>
+    <row r="71" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2519,8 +2650,9 @@
       <c r="R71" s="2"/>
       <c r="S71" s="2"/>
       <c r="T71" s="2"/>
-    </row>
-    <row r="72" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V71" s="2"/>
+    </row>
+    <row r="72" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2541,8 +2673,9 @@
       <c r="R72" s="2"/>
       <c r="S72" s="2"/>
       <c r="T72" s="2"/>
-    </row>
-    <row r="73" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V72" s="2"/>
+    </row>
+    <row r="73" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2563,8 +2696,9 @@
       <c r="R73" s="2"/>
       <c r="S73" s="2"/>
       <c r="T73" s="2"/>
-    </row>
-    <row r="74" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V73" s="2"/>
+    </row>
+    <row r="74" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2585,8 +2719,9 @@
       <c r="R74" s="2"/>
       <c r="S74" s="2"/>
       <c r="T74" s="2"/>
-    </row>
-    <row r="75" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V74" s="2"/>
+    </row>
+    <row r="75" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2607,8 +2742,9 @@
       <c r="R75" s="2"/>
       <c r="S75" s="2"/>
       <c r="T75" s="2"/>
-    </row>
-    <row r="76" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V75" s="2"/>
+    </row>
+    <row r="76" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2629,8 +2765,9 @@
       <c r="R76" s="2"/>
       <c r="S76" s="2"/>
       <c r="T76" s="2"/>
-    </row>
-    <row r="77" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V76" s="2"/>
+    </row>
+    <row r="77" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2651,8 +2788,9 @@
       <c r="R77" s="2"/>
       <c r="S77" s="2"/>
       <c r="T77" s="2"/>
-    </row>
-    <row r="78" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V77" s="2"/>
+    </row>
+    <row r="78" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2673,8 +2811,9 @@
       <c r="R78" s="2"/>
       <c r="S78" s="2"/>
       <c r="T78" s="2"/>
-    </row>
-    <row r="79" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V78" s="2"/>
+    </row>
+    <row r="79" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2695,8 +2834,9 @@
       <c r="R79" s="2"/>
       <c r="S79" s="2"/>
       <c r="T79" s="2"/>
-    </row>
-    <row r="80" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V79" s="2"/>
+    </row>
+    <row r="80" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2717,8 +2857,9 @@
       <c r="R80" s="2"/>
       <c r="S80" s="2"/>
       <c r="T80" s="2"/>
-    </row>
-    <row r="81" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V80" s="2"/>
+    </row>
+    <row r="81" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2739,8 +2880,9 @@
       <c r="R81" s="2"/>
       <c r="S81" s="2"/>
       <c r="T81" s="2"/>
-    </row>
-    <row r="82" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V81" s="2"/>
+    </row>
+    <row r="82" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2761,8 +2903,9 @@
       <c r="R82" s="2"/>
       <c r="S82" s="2"/>
       <c r="T82" s="2"/>
-    </row>
-    <row r="83" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V82" s="2"/>
+    </row>
+    <row r="83" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2783,8 +2926,9 @@
       <c r="R83" s="2"/>
       <c r="S83" s="2"/>
       <c r="T83" s="2"/>
-    </row>
-    <row r="84" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V83" s="2"/>
+    </row>
+    <row r="84" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2805,8 +2949,9 @@
       <c r="R84" s="2"/>
       <c r="S84" s="2"/>
       <c r="T84" s="2"/>
-    </row>
-    <row r="85" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V84" s="2"/>
+    </row>
+    <row r="85" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2827,8 +2972,9 @@
       <c r="R85" s="2"/>
       <c r="S85" s="2"/>
       <c r="T85" s="2"/>
-    </row>
-    <row r="86" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V85" s="2"/>
+    </row>
+    <row r="86" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2849,8 +2995,9 @@
       <c r="R86" s="2"/>
       <c r="S86" s="2"/>
       <c r="T86" s="2"/>
-    </row>
-    <row r="87" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V86" s="2"/>
+    </row>
+    <row r="87" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2871,8 +3018,9 @@
       <c r="R87" s="2"/>
       <c r="S87" s="2"/>
       <c r="T87" s="2"/>
-    </row>
-    <row r="88" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V87" s="2"/>
+    </row>
+    <row r="88" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2893,8 +3041,9 @@
       <c r="R88" s="2"/>
       <c r="S88" s="2"/>
       <c r="T88" s="2"/>
-    </row>
-    <row r="89" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V88" s="2"/>
+    </row>
+    <row r="89" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2915,8 +3064,9 @@
       <c r="R89" s="2"/>
       <c r="S89" s="2"/>
       <c r="T89" s="2"/>
-    </row>
-    <row r="90" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V89" s="2"/>
+    </row>
+    <row r="90" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2937,8 +3087,9 @@
       <c r="R90" s="2"/>
       <c r="S90" s="2"/>
       <c r="T90" s="2"/>
-    </row>
-    <row r="91" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V90" s="2"/>
+    </row>
+    <row r="91" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2959,8 +3110,9 @@
       <c r="R91" s="2"/>
       <c r="S91" s="2"/>
       <c r="T91" s="2"/>
-    </row>
-    <row r="92" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V91" s="2"/>
+    </row>
+    <row r="92" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2981,8 +3133,9 @@
       <c r="R92" s="2"/>
       <c r="S92" s="2"/>
       <c r="T92" s="2"/>
-    </row>
-    <row r="93" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V92" s="2"/>
+    </row>
+    <row r="93" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -3003,8 +3156,9 @@
       <c r="R93" s="2"/>
       <c r="S93" s="2"/>
       <c r="T93" s="2"/>
-    </row>
-    <row r="94" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V93" s="2"/>
+    </row>
+    <row r="94" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -3025,8 +3179,9 @@
       <c r="R94" s="2"/>
       <c r="S94" s="2"/>
       <c r="T94" s="2"/>
-    </row>
-    <row r="95" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V94" s="2"/>
+    </row>
+    <row r="95" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -3047,8 +3202,9 @@
       <c r="R95" s="2"/>
       <c r="S95" s="2"/>
       <c r="T95" s="2"/>
-    </row>
-    <row r="96" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V95" s="2"/>
+    </row>
+    <row r="96" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -3069,8 +3225,9 @@
       <c r="R96" s="2"/>
       <c r="S96" s="2"/>
       <c r="T96" s="2"/>
-    </row>
-    <row r="97" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V96" s="2"/>
+    </row>
+    <row r="97" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -3091,8 +3248,9 @@
       <c r="R97" s="2"/>
       <c r="S97" s="2"/>
       <c r="T97" s="2"/>
-    </row>
-    <row r="98" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V97" s="2"/>
+    </row>
+    <row r="98" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -3113,8 +3271,9 @@
       <c r="R98" s="2"/>
       <c r="S98" s="2"/>
       <c r="T98" s="2"/>
-    </row>
-    <row r="99" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V98" s="2"/>
+    </row>
+    <row r="99" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -3135,8 +3294,9 @@
       <c r="R99" s="2"/>
       <c r="S99" s="2"/>
       <c r="T99" s="2"/>
-    </row>
-    <row r="100" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V99" s="2"/>
+    </row>
+    <row r="100" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -3157,8 +3317,9 @@
       <c r="R100" s="2"/>
       <c r="S100" s="2"/>
       <c r="T100" s="2"/>
-    </row>
-    <row r="101" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V100" s="2"/>
+    </row>
+    <row r="101" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -3179,8 +3340,9 @@
       <c r="R101" s="2"/>
       <c r="S101" s="2"/>
       <c r="T101" s="2"/>
-    </row>
-    <row r="102" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V101" s="2"/>
+    </row>
+    <row r="102" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -3201,8 +3363,9 @@
       <c r="R102" s="2"/>
       <c r="S102" s="2"/>
       <c r="T102" s="2"/>
-    </row>
-    <row r="103" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V102" s="2"/>
+    </row>
+    <row r="103" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -3223,8 +3386,9 @@
       <c r="R103" s="2"/>
       <c r="S103" s="2"/>
       <c r="T103" s="2"/>
-    </row>
-    <row r="104" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V103" s="2"/>
+    </row>
+    <row r="104" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -3245,8 +3409,9 @@
       <c r="R104" s="2"/>
       <c r="S104" s="2"/>
       <c r="T104" s="2"/>
-    </row>
-    <row r="105" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V104" s="2"/>
+    </row>
+    <row r="105" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -3267,8 +3432,9 @@
       <c r="R105" s="2"/>
       <c r="S105" s="2"/>
       <c r="T105" s="2"/>
-    </row>
-    <row r="106" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V105" s="2"/>
+    </row>
+    <row r="106" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -3289,8 +3455,9 @@
       <c r="R106" s="2"/>
       <c r="S106" s="2"/>
       <c r="T106" s="2"/>
-    </row>
-    <row r="107" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V106" s="2"/>
+    </row>
+    <row r="107" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -3311,8 +3478,9 @@
       <c r="R107" s="2"/>
       <c r="S107" s="2"/>
       <c r="T107" s="2"/>
-    </row>
-    <row r="108" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V107" s="2"/>
+    </row>
+    <row r="108" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -3333,8 +3501,9 @@
       <c r="R108" s="2"/>
       <c r="S108" s="2"/>
       <c r="T108" s="2"/>
-    </row>
-    <row r="109" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V108" s="2"/>
+    </row>
+    <row r="109" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -3355,8 +3524,9 @@
       <c r="R109" s="2"/>
       <c r="S109" s="2"/>
       <c r="T109" s="2"/>
-    </row>
-    <row r="110" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V109" s="2"/>
+    </row>
+    <row r="110" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -3377,8 +3547,9 @@
       <c r="R110" s="2"/>
       <c r="S110" s="2"/>
       <c r="T110" s="2"/>
-    </row>
-    <row r="111" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V110" s="2"/>
+    </row>
+    <row r="111" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -3399,8 +3570,9 @@
       <c r="R111" s="2"/>
       <c r="S111" s="2"/>
       <c r="T111" s="2"/>
-    </row>
-    <row r="112" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V111" s="2"/>
+    </row>
+    <row r="112" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -3421,8 +3593,9 @@
       <c r="R112" s="2"/>
       <c r="S112" s="2"/>
       <c r="T112" s="2"/>
-    </row>
-    <row r="113" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V112" s="2"/>
+    </row>
+    <row r="113" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -3443,8 +3616,9 @@
       <c r="R113" s="2"/>
       <c r="S113" s="2"/>
       <c r="T113" s="2"/>
-    </row>
-    <row r="114" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V113" s="2"/>
+    </row>
+    <row r="114" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -3465,8 +3639,9 @@
       <c r="R114" s="2"/>
       <c r="S114" s="2"/>
       <c r="T114" s="2"/>
-    </row>
-    <row r="115" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V114" s="2"/>
+    </row>
+    <row r="115" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -3487,8 +3662,9 @@
       <c r="R115" s="2"/>
       <c r="S115" s="2"/>
       <c r="T115" s="2"/>
-    </row>
-    <row r="116" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V115" s="2"/>
+    </row>
+    <row r="116" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -3509,8 +3685,9 @@
       <c r="R116" s="2"/>
       <c r="S116" s="2"/>
       <c r="T116" s="2"/>
-    </row>
-    <row r="117" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V116" s="2"/>
+    </row>
+    <row r="117" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -3531,8 +3708,9 @@
       <c r="R117" s="2"/>
       <c r="S117" s="2"/>
       <c r="T117" s="2"/>
-    </row>
-    <row r="118" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V117" s="2"/>
+    </row>
+    <row r="118" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -3553,8 +3731,9 @@
       <c r="R118" s="2"/>
       <c r="S118" s="2"/>
       <c r="T118" s="2"/>
-    </row>
-    <row r="119" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V118" s="2"/>
+    </row>
+    <row r="119" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -3575,8 +3754,9 @@
       <c r="R119" s="2"/>
       <c r="S119" s="2"/>
       <c r="T119" s="2"/>
-    </row>
-    <row r="120" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V119" s="2"/>
+    </row>
+    <row r="120" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -3597,8 +3777,9 @@
       <c r="R120" s="2"/>
       <c r="S120" s="2"/>
       <c r="T120" s="2"/>
-    </row>
-    <row r="121" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V120" s="2"/>
+    </row>
+    <row r="121" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -3619,8 +3800,9 @@
       <c r="R121" s="2"/>
       <c r="S121" s="2"/>
       <c r="T121" s="2"/>
-    </row>
-    <row r="122" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V121" s="2"/>
+    </row>
+    <row r="122" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -3641,8 +3823,9 @@
       <c r="R122" s="2"/>
       <c r="S122" s="2"/>
       <c r="T122" s="2"/>
-    </row>
-    <row r="123" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V122" s="2"/>
+    </row>
+    <row r="123" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -3663,8 +3846,9 @@
       <c r="R123" s="2"/>
       <c r="S123" s="2"/>
       <c r="T123" s="2"/>
-    </row>
-    <row r="124" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V123" s="2"/>
+    </row>
+    <row r="124" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -3685,8 +3869,9 @@
       <c r="R124" s="2"/>
       <c r="S124" s="2"/>
       <c r="T124" s="2"/>
-    </row>
-    <row r="125" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V124" s="2"/>
+    </row>
+    <row r="125" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -3707,8 +3892,9 @@
       <c r="R125" s="2"/>
       <c r="S125" s="2"/>
       <c r="T125" s="2"/>
-    </row>
-    <row r="126" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V125" s="2"/>
+    </row>
+    <row r="126" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -3729,8 +3915,9 @@
       <c r="R126" s="2"/>
       <c r="S126" s="2"/>
       <c r="T126" s="2"/>
-    </row>
-    <row r="127" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V126" s="2"/>
+    </row>
+    <row r="127" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -3751,8 +3938,9 @@
       <c r="R127" s="2"/>
       <c r="S127" s="2"/>
       <c r="T127" s="2"/>
-    </row>
-    <row r="128" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V127" s="2"/>
+    </row>
+    <row r="128" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -3773,8 +3961,9 @@
       <c r="R128" s="2"/>
       <c r="S128" s="2"/>
       <c r="T128" s="2"/>
-    </row>
-    <row r="129" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V128" s="2"/>
+    </row>
+    <row r="129" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -3795,8 +3984,9 @@
       <c r="R129" s="2"/>
       <c r="S129" s="2"/>
       <c r="T129" s="2"/>
-    </row>
-    <row r="130" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V129" s="2"/>
+    </row>
+    <row r="130" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -3817,8 +4007,9 @@
       <c r="R130" s="2"/>
       <c r="S130" s="2"/>
       <c r="T130" s="2"/>
-    </row>
-    <row r="131" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V130" s="2"/>
+    </row>
+    <row r="131" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -3839,8 +4030,9 @@
       <c r="R131" s="2"/>
       <c r="S131" s="2"/>
       <c r="T131" s="2"/>
-    </row>
-    <row r="132" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V131" s="2"/>
+    </row>
+    <row r="132" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -3861,8 +4053,9 @@
       <c r="R132" s="2"/>
       <c r="S132" s="2"/>
       <c r="T132" s="2"/>
-    </row>
-    <row r="133" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V132" s="2"/>
+    </row>
+    <row r="133" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -3883,8 +4076,9 @@
       <c r="R133" s="2"/>
       <c r="S133" s="2"/>
       <c r="T133" s="2"/>
-    </row>
-    <row r="134" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V133" s="2"/>
+    </row>
+    <row r="134" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -3905,8 +4099,9 @@
       <c r="R134" s="2"/>
       <c r="S134" s="2"/>
       <c r="T134" s="2"/>
-    </row>
-    <row r="135" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V134" s="2"/>
+    </row>
+    <row r="135" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -3927,8 +4122,9 @@
       <c r="R135" s="2"/>
       <c r="S135" s="2"/>
       <c r="T135" s="2"/>
-    </row>
-    <row r="136" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V135" s="2"/>
+    </row>
+    <row r="136" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -3949,8 +4145,9 @@
       <c r="R136" s="2"/>
       <c r="S136" s="2"/>
       <c r="T136" s="2"/>
-    </row>
-    <row r="137" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V136" s="2"/>
+    </row>
+    <row r="137" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -3971,8 +4168,9 @@
       <c r="R137" s="2"/>
       <c r="S137" s="2"/>
       <c r="T137" s="2"/>
-    </row>
-    <row r="138" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V137" s="2"/>
+    </row>
+    <row r="138" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -3993,8 +4191,9 @@
       <c r="R138" s="2"/>
       <c r="S138" s="2"/>
       <c r="T138" s="2"/>
-    </row>
-    <row r="139" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V138" s="2"/>
+    </row>
+    <row r="139" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -4015,8 +4214,9 @@
       <c r="R139" s="2"/>
       <c r="S139" s="2"/>
       <c r="T139" s="2"/>
-    </row>
-    <row r="140" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V139" s="2"/>
+    </row>
+    <row r="140" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -4037,8 +4237,9 @@
       <c r="R140" s="2"/>
       <c r="S140" s="2"/>
       <c r="T140" s="2"/>
-    </row>
-    <row r="141" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V140" s="2"/>
+    </row>
+    <row r="141" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -4059,8 +4260,9 @@
       <c r="R141" s="2"/>
       <c r="S141" s="2"/>
       <c r="T141" s="2"/>
-    </row>
-    <row r="142" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V141" s="2"/>
+    </row>
+    <row r="142" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -4081,8 +4283,9 @@
       <c r="R142" s="2"/>
       <c r="S142" s="2"/>
       <c r="T142" s="2"/>
-    </row>
-    <row r="143" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V142" s="2"/>
+    </row>
+    <row r="143" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -4103,8 +4306,9 @@
       <c r="R143" s="2"/>
       <c r="S143" s="2"/>
       <c r="T143" s="2"/>
-    </row>
-    <row r="144" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V143" s="2"/>
+    </row>
+    <row r="144" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -4125,8 +4329,9 @@
       <c r="R144" s="2"/>
       <c r="S144" s="2"/>
       <c r="T144" s="2"/>
-    </row>
-    <row r="145" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V144" s="2"/>
+    </row>
+    <row r="145" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -4147,8 +4352,9 @@
       <c r="R145" s="2"/>
       <c r="S145" s="2"/>
       <c r="T145" s="2"/>
-    </row>
-    <row r="146" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V145" s="2"/>
+    </row>
+    <row r="146" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -4169,8 +4375,9 @@
       <c r="R146" s="2"/>
       <c r="S146" s="2"/>
       <c r="T146" s="2"/>
-    </row>
-    <row r="147" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V146" s="2"/>
+    </row>
+    <row r="147" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -4191,8 +4398,9 @@
       <c r="R147" s="2"/>
       <c r="S147" s="2"/>
       <c r="T147" s="2"/>
-    </row>
-    <row r="148" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V147" s="2"/>
+    </row>
+    <row r="148" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -4213,8 +4421,9 @@
       <c r="R148" s="2"/>
       <c r="S148" s="2"/>
       <c r="T148" s="2"/>
-    </row>
-    <row r="149" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V148" s="2"/>
+    </row>
+    <row r="149" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -4235,8 +4444,9 @@
       <c r="R149" s="2"/>
       <c r="S149" s="2"/>
       <c r="T149" s="2"/>
-    </row>
-    <row r="150" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V149" s="2"/>
+    </row>
+    <row r="150" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -4257,8 +4467,9 @@
       <c r="R150" s="2"/>
       <c r="S150" s="2"/>
       <c r="T150" s="2"/>
-    </row>
-    <row r="151" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V150" s="2"/>
+    </row>
+    <row r="151" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -4279,8 +4490,9 @@
       <c r="R151" s="2"/>
       <c r="S151" s="2"/>
       <c r="T151" s="2"/>
-    </row>
-    <row r="152" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V151" s="2"/>
+    </row>
+    <row r="152" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -4301,8 +4513,9 @@
       <c r="R152" s="2"/>
       <c r="S152" s="2"/>
       <c r="T152" s="2"/>
-    </row>
-    <row r="153" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V152" s="2"/>
+    </row>
+    <row r="153" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -4323,8 +4536,9 @@
       <c r="R153" s="2"/>
       <c r="S153" s="2"/>
       <c r="T153" s="2"/>
-    </row>
-    <row r="154" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V153" s="2"/>
+    </row>
+    <row r="154" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -4345,8 +4559,9 @@
       <c r="R154" s="2"/>
       <c r="S154" s="2"/>
       <c r="T154" s="2"/>
-    </row>
-    <row r="155" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V154" s="2"/>
+    </row>
+    <row r="155" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -4367,8 +4582,9 @@
       <c r="R155" s="2"/>
       <c r="S155" s="2"/>
       <c r="T155" s="2"/>
-    </row>
-    <row r="156" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V155" s="2"/>
+    </row>
+    <row r="156" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A156" s="2"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -4389,8 +4605,9 @@
       <c r="R156" s="2"/>
       <c r="S156" s="2"/>
       <c r="T156" s="2"/>
-    </row>
-    <row r="157" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V156" s="2"/>
+    </row>
+    <row r="157" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A157" s="2"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -4411,8 +4628,9 @@
       <c r="R157" s="2"/>
       <c r="S157" s="2"/>
       <c r="T157" s="2"/>
-    </row>
-    <row r="158" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="V157" s="2"/>
+    </row>
+    <row r="158" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -4433,8 +4651,9 @@
       <c r="R158" s="2"/>
       <c r="S158" s="2"/>
       <c r="T158" s="2"/>
-    </row>
-    <row r="159" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="V158" s="2"/>
+    </row>
+    <row r="159" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A159" s="2"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -4456,7 +4675,7 @@
       <c r="S159" s="1"/>
       <c r="T159" s="1"/>
     </row>
-    <row r="160" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A160" s="2"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -4478,7 +4697,7 @@
       <c r="S160" s="1"/>
       <c r="T160" s="1"/>
     </row>
-    <row r="161" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A161" s="2"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -4500,7 +4719,7 @@
       <c r="S161" s="1"/>
       <c r="T161" s="1"/>
     </row>
-    <row r="162" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A162" s="2"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -4522,7 +4741,7 @@
       <c r="S162" s="1"/>
       <c r="T162" s="1"/>
     </row>
-    <row r="163" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A163" s="2"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -4544,7 +4763,7 @@
       <c r="S163" s="1"/>
       <c r="T163" s="1"/>
     </row>
-    <row r="164" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A164" s="2"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -4566,7 +4785,7 @@
       <c r="S164" s="1"/>
       <c r="T164" s="1"/>
     </row>
-    <row r="165" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A165" s="2"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -4588,7 +4807,7 @@
       <c r="S165" s="1"/>
       <c r="T165" s="1"/>
     </row>
-    <row r="166" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A166" s="2"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -4611,23 +4830,11 @@
       <c r="T166" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="R19:S19"/>
+  <mergeCells count="38">
+    <mergeCell ref="V4:V5"/>
+    <mergeCell ref="V9:V11"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="Q20:S20"/>
     <mergeCell ref="O16:S16"/>
     <mergeCell ref="T4:T21"/>
     <mergeCell ref="B21:S21"/>
@@ -4644,6 +4851,20 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D4:S5"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="E11:F11"/>
     <mergeCell ref="E6:S8"/>
     <mergeCell ref="G9:S11"/>
     <mergeCell ref="B6:B8"/>

</xml_diff>